<commit_message>
Se agrega prueba con grado 10000
</commit_message>
<xml_diff>
--- a/Documentación/Rendimiento.xlsx
+++ b/Documentación/Rendimiento.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="15">
   <si>
     <t>Recursiva</t>
   </si>
@@ -58,6 +58,9 @@
   </si>
   <si>
     <t>Complejidad O(n.long(n))</t>
+  </si>
+  <si>
+    <t>Rompe</t>
   </si>
 </sst>
 </file>
@@ -405,7 +408,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -445,6 +448,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="23" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="24" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -503,7 +507,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Alg 2,1'!$B$19</c:f>
+              <c:f>'Alg 2,1'!$B$20</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -517,15 +521,15 @@
           </c:marker>
           <c:trendline>
             <c:trendlineType val="poly"/>
-            <c:order val="5"/>
+            <c:order val="6"/>
             <c:dispRSqr val="0"/>
             <c:dispEq val="0"/>
           </c:trendline>
           <c:cat>
             <c:strRef>
-              <c:f>'Alg 2,1'!$A$19:$A$31</c:f>
+              <c:f>'Alg 2,1'!$A$20:$A$33</c:f>
               <c:strCache>
-                <c:ptCount val="13"/>
+                <c:ptCount val="14"/>
                 <c:pt idx="0">
                   <c:v>Grado</c:v>
                 </c:pt>
@@ -564,44 +568,56 @@
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>5000</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>10000</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Alg 2,1'!$B$22:$B$31</c:f>
+              <c:f>'Alg 2,1'!$B$20:$B$32</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="13"/>
                 <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>2</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="3">
                   <c:v>2</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="4">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>4</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="6">
                   <c:v>6</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="7">
                   <c:v>8</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="8">
                   <c:v>13</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="9">
                   <c:v>19</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="10">
                   <c:v>24</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="11">
                   <c:v>35</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="12">
                   <c:v>100</c:v>
                 </c:pt>
               </c:numCache>
@@ -619,11 +635,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="86476672"/>
-        <c:axId val="86478208"/>
+        <c:axId val="88239104"/>
+        <c:axId val="88240896"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="86476672"/>
+        <c:axId val="88239104"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -632,7 +648,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="86478208"/>
+        <c:crossAx val="88240896"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -640,7 +656,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="86478208"/>
+        <c:axId val="88240896"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -651,7 +667,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="86476672"/>
+        <c:crossAx val="88239104"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -717,7 +733,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Alg 2,1'!$B$34</c:f>
+              <c:f>'Alg 2,1'!$B$36</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -731,15 +747,15 @@
           </c:marker>
           <c:trendline>
             <c:trendlineType val="poly"/>
-            <c:order val="5"/>
+            <c:order val="4"/>
             <c:dispRSqr val="0"/>
             <c:dispEq val="0"/>
           </c:trendline>
           <c:cat>
             <c:strRef>
-              <c:f>'Alg 2,1'!$A$34:$A$46</c:f>
+              <c:f>'Alg 2,1'!$A$36:$A$49</c:f>
               <c:strCache>
-                <c:ptCount val="13"/>
+                <c:ptCount val="14"/>
                 <c:pt idx="0">
                   <c:v>Grado</c:v>
                 </c:pt>
@@ -778,45 +794,57 @@
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>5000</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>10000</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Alg 2,1'!$B$37:$B$46</c:f>
+              <c:f>'Alg 2,1'!$B$37:$B$49</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="13"/>
                 <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>2</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>3</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="4">
                   <c:v>5</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="5">
                   <c:v>7</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="6">
                   <c:v>8</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="7">
                   <c:v>14</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="8">
                   <c:v>20</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="9">
                   <c:v>25</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="10">
                   <c:v>36</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="11">
                   <c:v>102</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>108</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -833,11 +861,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="93090944"/>
-        <c:axId val="93092480"/>
+        <c:axId val="88262144"/>
+        <c:axId val="88263680"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="93090944"/>
+        <c:axId val="88262144"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -846,7 +874,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="93092480"/>
+        <c:crossAx val="88263680"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -854,7 +882,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="93092480"/>
+        <c:axId val="88263680"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -865,7 +893,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="93090944"/>
+        <c:crossAx val="88262144"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -931,7 +959,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Alg 2,1'!$B$49</c:f>
+              <c:f>'Alg 2,1'!$B$52</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -945,15 +973,15 @@
           </c:marker>
           <c:trendline>
             <c:trendlineType val="poly"/>
-            <c:order val="5"/>
+            <c:order val="4"/>
             <c:dispRSqr val="0"/>
             <c:dispEq val="0"/>
           </c:trendline>
           <c:cat>
             <c:strRef>
-              <c:f>'Alg 2,1'!$A$49:$A$61</c:f>
+              <c:f>'Alg 2,1'!$A$52:$A$65</c:f>
               <c:strCache>
-                <c:ptCount val="13"/>
+                <c:ptCount val="14"/>
                 <c:pt idx="0">
                   <c:v>Grado</c:v>
                 </c:pt>
@@ -992,45 +1020,60 @@
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>5000</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>10000</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Alg 2,1'!$B$52:$B$61</c:f>
+              <c:f>'Alg 2,1'!$B$52:$B$65</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="14"/>
                 <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>3</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="4">
                   <c:v>3</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="5">
                   <c:v>5</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="6">
                   <c:v>7</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="7">
                   <c:v>9</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="8">
                   <c:v>15</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="9">
                   <c:v>21</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="10">
                   <c:v>25</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="11">
                   <c:v>36</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="12">
                   <c:v>103</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>109</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1047,11 +1090,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="102791040"/>
-        <c:axId val="104558592"/>
+        <c:axId val="88297472"/>
+        <c:axId val="88299008"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="102791040"/>
+        <c:axId val="88297472"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1060,7 +1103,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="104558592"/>
+        <c:crossAx val="88299008"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1068,7 +1111,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="104558592"/>
+        <c:axId val="88299008"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1079,7 +1122,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="102791040"/>
+        <c:crossAx val="88297472"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1145,7 +1188,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Alg 2,1'!$B$64</c:f>
+              <c:f>'Alg 2,1'!$B$68</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1159,15 +1202,15 @@
           </c:marker>
           <c:trendline>
             <c:trendlineType val="poly"/>
-            <c:order val="6"/>
+            <c:order val="4"/>
             <c:dispRSqr val="0"/>
             <c:dispEq val="0"/>
           </c:trendline>
           <c:cat>
             <c:strRef>
-              <c:f>'Alg 2,1'!$A$64:$A$76</c:f>
+              <c:f>'Alg 2,1'!$A$68:$A$81</c:f>
               <c:strCache>
-                <c:ptCount val="13"/>
+                <c:ptCount val="14"/>
                 <c:pt idx="0">
                   <c:v>Grado</c:v>
                 </c:pt>
@@ -1206,45 +1249,60 @@
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>5000</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>10000</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Alg 2,1'!$B$67:$B$76</c:f>
+              <c:f>'Alg 2,1'!$B$68:$B$81</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="14"/>
                 <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>3</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="4">
                   <c:v>3</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="5">
                   <c:v>5</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="6">
                   <c:v>7</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="7">
                   <c:v>9</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="8">
                   <c:v>16</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="9">
                   <c:v>21</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="10">
                   <c:v>25</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="11">
                   <c:v>37</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="12">
                   <c:v>103</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>109</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1261,11 +1319,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="86942464"/>
-        <c:axId val="86944000"/>
+        <c:axId val="88320256"/>
+        <c:axId val="88326144"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="86942464"/>
+        <c:axId val="88320256"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1274,7 +1332,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="86944000"/>
+        <c:crossAx val="88326144"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1282,7 +1340,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="86944000"/>
+        <c:axId val="88326144"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1293,7 +1351,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="86942464"/>
+        <c:crossAx val="88320256"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1359,7 +1417,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Alg 2,1'!$B$94</c:f>
+              <c:f>'Alg 2,1'!$B$100</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1373,45 +1431,104 @@
           </c:marker>
           <c:trendline>
             <c:trendlineType val="poly"/>
-            <c:order val="6"/>
+            <c:order val="4"/>
             <c:dispRSqr val="0"/>
             <c:dispEq val="0"/>
           </c:trendline>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Alg 2,1'!$A$100:$A$113</c:f>
+              <c:strCache>
+                <c:ptCount val="14"/>
+                <c:pt idx="0">
+                  <c:v>Grado</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>300</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>750</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1500</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2000</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2500</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>5000</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>10000</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Alg 2,1'!$B$97:$B$106</c:f>
+              <c:f>'Alg 2,1'!$B$101:$B$113</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="13"/>
                 <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>3</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="3">
                   <c:v>3</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="4">
                   <c:v>5</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="5">
                   <c:v>9</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="6">
                   <c:v>9</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="7">
                   <c:v>17</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="8">
                   <c:v>22</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="9">
                   <c:v>27</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="10">
                   <c:v>38</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="11">
                   <c:v>106</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>115</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1428,11 +1545,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="86456192"/>
-        <c:axId val="86498688"/>
+        <c:axId val="89002752"/>
+        <c:axId val="89004288"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="86456192"/>
+        <c:axId val="89002752"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1441,7 +1558,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="86498688"/>
+        <c:crossAx val="89004288"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1449,7 +1566,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="86498688"/>
+        <c:axId val="89004288"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1460,7 +1577,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="86456192"/>
+        <c:crossAx val="89002752"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1526,7 +1643,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Alg 2,1'!$B$79</c:f>
+              <c:f>'Alg 2,1'!$B$84</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1540,45 +1657,107 @@
           </c:marker>
           <c:trendline>
             <c:trendlineType val="poly"/>
-            <c:order val="6"/>
+            <c:order val="4"/>
             <c:dispRSqr val="0"/>
             <c:dispEq val="0"/>
           </c:trendline>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Alg 2,1'!$A$84:$A$97</c:f>
+              <c:strCache>
+                <c:ptCount val="14"/>
+                <c:pt idx="0">
+                  <c:v>Grado</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>300</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>750</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1500</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2000</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2500</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>5000</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>10000</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Alg 2,1'!$B$82:$B$91</c:f>
+              <c:f>'Alg 2,1'!$B$84:$B$97</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="14"/>
                 <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>3</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="4">
                   <c:v>3</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="5">
                   <c:v>5</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="6">
                   <c:v>9</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="7">
                   <c:v>9</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="8">
                   <c:v>16</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="9">
                   <c:v>22</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="10">
                   <c:v>27</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="11">
                   <c:v>38</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="12">
                   <c:v>106</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>115</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1595,11 +1774,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="93071232"/>
-        <c:axId val="102238848"/>
+        <c:axId val="89086976"/>
+        <c:axId val="89088768"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="93071232"/>
+        <c:axId val="89086976"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1608,7 +1787,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="102238848"/>
+        <c:crossAx val="89088768"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1616,7 +1795,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="102238848"/>
+        <c:axId val="89088768"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1627,7 +1806,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="93071232"/>
+        <c:crossAx val="89086976"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1718,9 +1897,9 @@
           </c:trendline>
           <c:cat>
             <c:strRef>
-              <c:f>'Alg 2,1'!$A$4:$A$16</c:f>
+              <c:f>'Alg 2,1'!$A$4:$A$17</c:f>
               <c:strCache>
-                <c:ptCount val="13"/>
+                <c:ptCount val="14"/>
                 <c:pt idx="0">
                   <c:v>Grado</c:v>
                 </c:pt>
@@ -1759,16 +1938,19 @@
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>5000</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>10000</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Alg 2,1'!$B$5:$B$16</c:f>
+              <c:f>'Alg 2,1'!$B$5:$B$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="12"/>
+                <c:ptCount val="13"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -1804,6 +1986,9 @@
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>102</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1820,11 +2005,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="102851712"/>
-        <c:axId val="102854016"/>
+        <c:axId val="89126400"/>
+        <c:axId val="89127936"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="102851712"/>
+        <c:axId val="89126400"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1833,7 +2018,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="102854016"/>
+        <c:crossAx val="89127936"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1841,7 +2026,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="102854016"/>
+        <c:axId val="89127936"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1852,7 +2037,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="102851712"/>
+        <c:crossAx val="89126400"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1879,15 +2064,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>28574</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>185737</xdr:rowOff>
+      <xdr:colOff>9524</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>33337</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>238124</xdr:colOff>
-      <xdr:row>31</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
+      <xdr:colOff>219074</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1908,16 +2093,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>857250</xdr:colOff>
-      <xdr:row>32</xdr:row>
-      <xdr:rowOff>4762</xdr:rowOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>23812</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>476250</xdr:colOff>
-      <xdr:row>46</xdr:row>
-      <xdr:rowOff>57150</xdr:rowOff>
+      <xdr:colOff>495300</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1939,15 +2124,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>19050</xdr:colOff>
-      <xdr:row>47</xdr:row>
-      <xdr:rowOff>4760</xdr:rowOff>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>90485</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>266700</xdr:colOff>
-      <xdr:row>61</xdr:row>
-      <xdr:rowOff>47624</xdr:rowOff>
+      <xdr:colOff>257175</xdr:colOff>
+      <xdr:row>64</xdr:row>
+      <xdr:rowOff>133349</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1969,15 +2154,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>28574</xdr:colOff>
-      <xdr:row>61</xdr:row>
-      <xdr:rowOff>157162</xdr:rowOff>
+      <xdr:colOff>19049</xdr:colOff>
+      <xdr:row>66</xdr:row>
+      <xdr:rowOff>52387</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>28574</xdr:colOff>
-      <xdr:row>76</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:colOff>19049</xdr:colOff>
+      <xdr:row>80</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1999,15 +2184,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>761999</xdr:colOff>
-      <xdr:row>92</xdr:row>
-      <xdr:rowOff>33337</xdr:rowOff>
+      <xdr:colOff>752474</xdr:colOff>
+      <xdr:row>98</xdr:row>
+      <xdr:rowOff>61912</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>619124</xdr:colOff>
-      <xdr:row>106</xdr:row>
-      <xdr:rowOff>47625</xdr:rowOff>
+      <xdr:colOff>609599</xdr:colOff>
+      <xdr:row>112</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2028,16 +2213,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>9525</xdr:colOff>
-      <xdr:row>76</xdr:row>
-      <xdr:rowOff>147637</xdr:rowOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>781050</xdr:colOff>
+      <xdr:row>81</xdr:row>
+      <xdr:rowOff>128587</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>28575</xdr:colOff>
-      <xdr:row>91</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>695325</xdr:colOff>
+      <xdr:row>96</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2376,10 +2561,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D106"/>
+  <dimension ref="A1:D113"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A91" workbookViewId="0">
-      <selection activeCell="K25" sqref="K25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="P112" sqref="P112"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2516,44 +2701,44 @@
         <v>28</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="33" t="s">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>10000</v>
+      </c>
+      <c r="B17" s="39">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="33" t="s">
         <v>0</v>
       </c>
-      <c r="B18" s="34" t="s">
+      <c r="B19" s="34" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="37" t="s">
+      <c r="C19" s="36"/>
+    </row>
+    <row r="20" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="37" t="s">
         <v>6</v>
       </c>
-      <c r="B19" s="38" t="s">
+      <c r="B20" s="38" t="s">
         <v>7</v>
-      </c>
-      <c r="C19" s="36"/>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="35">
-        <v>2</v>
-      </c>
-      <c r="B20" s="35">
-        <v>1</v>
       </c>
       <c r="C20" s="36"/>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="35">
-        <v>50</v>
+        <v>2</v>
       </c>
       <c r="B21" s="35">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C21" s="36"/>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="35">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="B22" s="35">
         <v>2</v>
@@ -2562,7 +2747,7 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="35">
-        <v>150</v>
+        <v>100</v>
       </c>
       <c r="B23" s="35">
         <v>2</v>
@@ -2571,632 +2756,688 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="35">
-        <v>300</v>
+        <v>150</v>
       </c>
       <c r="B24" s="35">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C24" s="36"/>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="35">
-        <v>500</v>
+        <v>300</v>
       </c>
       <c r="B25" s="35">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C25" s="36"/>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="35">
-        <v>750</v>
+        <v>500</v>
       </c>
       <c r="B26" s="35">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C26" s="36"/>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="35">
-        <v>1000</v>
+        <v>750</v>
       </c>
       <c r="B27" s="35">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="C27" s="36"/>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="35">
-        <v>1500</v>
+        <v>1000</v>
       </c>
       <c r="B28" s="35">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="C28" s="36"/>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="35">
-        <v>2000</v>
+        <v>1500</v>
       </c>
       <c r="B29" s="35">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="C29" s="36"/>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="35">
-        <v>2500</v>
+        <v>2000</v>
       </c>
       <c r="B30" s="35">
-        <v>35</v>
+        <v>24</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="35">
+        <v>2500</v>
+      </c>
+      <c r="B31" s="35">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" s="35">
         <v>5000</v>
       </c>
-      <c r="B31" s="35">
+      <c r="B32" s="35">
         <v>100</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A33" s="27" t="s">
+      <c r="A33" s="35">
+        <v>10000</v>
+      </c>
+      <c r="B33" s="35" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="B33" s="28" t="s">
+      <c r="B35" s="28" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="34" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="29" t="s">
+    <row r="36" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="29" t="s">
         <v>6</v>
       </c>
-      <c r="B34" s="30" t="s">
+      <c r="B36" s="30" t="s">
         <v>7</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A35" s="31">
-        <v>2</v>
-      </c>
-      <c r="B35" s="32">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A36" s="31">
-        <v>50</v>
-      </c>
-      <c r="B36" s="32">
-        <v>2</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" s="31">
-        <v>100</v>
+        <v>2</v>
       </c>
       <c r="B37" s="32">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" s="31">
-        <v>150</v>
+        <v>50</v>
       </c>
       <c r="B38" s="32">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" s="31">
-        <v>300</v>
+        <v>100</v>
       </c>
       <c r="B39" s="32">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" s="31">
-        <v>500</v>
+        <v>150</v>
       </c>
       <c r="B40" s="32">
-        <v>7</v>
+        <v>3</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" s="31">
-        <v>750</v>
+        <v>300</v>
       </c>
       <c r="B41" s="32">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" s="31">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="B42" s="32">
-        <v>14</v>
+        <v>7</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" s="31">
-        <v>1500</v>
+        <v>750</v>
       </c>
       <c r="B43" s="32">
-        <v>20</v>
+        <v>8</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" s="31">
-        <v>2000</v>
+        <v>1000</v>
       </c>
       <c r="B44" s="32">
-        <v>25</v>
+        <v>14</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" s="31">
-        <v>2500</v>
+        <v>1500</v>
       </c>
       <c r="B45" s="32">
-        <v>36</v>
+        <v>20</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" s="31">
+        <v>2000</v>
+      </c>
+      <c r="B46" s="32">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A47" s="31">
+        <v>2500</v>
+      </c>
+      <c r="B47" s="32">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A48" s="31">
         <v>5000</v>
       </c>
-      <c r="B46" s="32">
+      <c r="B48" s="32">
         <v>102</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A48" s="21" t="s">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49" s="31">
+        <v>10000</v>
+      </c>
+      <c r="B49" s="32">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A51" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="B48" s="22" t="s">
+      <c r="B51" s="22" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="49" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="25" t="s">
+    <row r="52" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A52" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="B49" s="26" t="s">
+      <c r="B52" s="26" t="s">
         <v>7</v>
-      </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A50" s="23">
-        <v>2</v>
-      </c>
-      <c r="B50" s="24">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A51" s="23">
-        <v>50</v>
-      </c>
-      <c r="B51" s="24">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A52" s="23">
-        <v>100</v>
-      </c>
-      <c r="B52" s="24">
-        <v>3</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" s="23">
-        <v>150</v>
+        <v>2</v>
       </c>
       <c r="B53" s="24">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" s="23">
-        <v>300</v>
+        <v>50</v>
       </c>
       <c r="B54" s="24">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" s="23">
-        <v>500</v>
+        <v>100</v>
       </c>
       <c r="B55" s="24">
-        <v>7</v>
+        <v>3</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" s="23">
-        <v>750</v>
+        <v>150</v>
       </c>
       <c r="B56" s="24">
-        <v>9</v>
+        <v>3</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" s="23">
-        <v>1000</v>
+        <v>300</v>
       </c>
       <c r="B57" s="24">
-        <v>15</v>
+        <v>5</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" s="23">
-        <v>1500</v>
+        <v>500</v>
       </c>
       <c r="B58" s="24">
-        <v>21</v>
+        <v>7</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" s="23">
-        <v>2000</v>
+        <v>750</v>
       </c>
       <c r="B59" s="24">
-        <v>25</v>
+        <v>9</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" s="23">
-        <v>2500</v>
+        <v>1000</v>
       </c>
       <c r="B60" s="24">
-        <v>36</v>
+        <v>15</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61" s="23">
+        <v>1500</v>
+      </c>
+      <c r="B61" s="24">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A62" s="23">
+        <v>2000</v>
+      </c>
+      <c r="B62" s="24">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A63" s="23">
+        <v>2500</v>
+      </c>
+      <c r="B63" s="24">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A64" s="23">
         <v>5000</v>
       </c>
-      <c r="B61" s="24">
+      <c r="B64" s="24">
         <v>103</v>
       </c>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A63" s="15" t="s">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A65" s="23">
+        <v>10000</v>
+      </c>
+      <c r="B65" s="24">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A67" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="B63" s="16" t="s">
+      <c r="B67" s="16" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="64" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A64" s="19" t="s">
+    <row r="68" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A68" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="B64" s="20" t="s">
+      <c r="B68" s="20" t="s">
         <v>7</v>
-      </c>
-    </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A65" s="17">
-        <v>2</v>
-      </c>
-      <c r="B65" s="18">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A66" s="17">
-        <v>50</v>
-      </c>
-      <c r="B66" s="18">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A67" s="17">
-        <v>100</v>
-      </c>
-      <c r="B67" s="18">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A68" s="17">
-        <v>150</v>
-      </c>
-      <c r="B68" s="18">
-        <v>3</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69" s="17">
-        <v>300</v>
+        <v>2</v>
       </c>
       <c r="B69" s="18">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70" s="17">
-        <v>500</v>
+        <v>50</v>
       </c>
       <c r="B70" s="18">
-        <v>7</v>
+        <v>2</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71" s="17">
-        <v>750</v>
+        <v>100</v>
       </c>
       <c r="B71" s="18">
-        <v>9</v>
+        <v>3</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72" s="17">
-        <v>1000</v>
+        <v>150</v>
       </c>
       <c r="B72" s="18">
-        <v>16</v>
+        <v>3</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73" s="17">
-        <v>1500</v>
+        <v>300</v>
       </c>
       <c r="B73" s="18">
-        <v>21</v>
+        <v>5</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A74" s="17">
-        <v>2000</v>
+        <v>500</v>
       </c>
       <c r="B74" s="18">
-        <v>25</v>
+        <v>7</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A75" s="17">
-        <v>2500</v>
+        <v>750</v>
       </c>
       <c r="B75" s="18">
-        <v>37</v>
+        <v>9</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A76" s="17">
+        <v>1000</v>
+      </c>
+      <c r="B76" s="18">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A77" s="17">
+        <v>1500</v>
+      </c>
+      <c r="B77" s="18">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A78" s="17">
+        <v>2000</v>
+      </c>
+      <c r="B78" s="18">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A79" s="17">
+        <v>2500</v>
+      </c>
+      <c r="B79" s="18">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A80" s="17">
         <v>5000</v>
       </c>
-      <c r="B76" s="18">
+      <c r="B80" s="18">
         <v>103</v>
       </c>
     </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A78" s="9" t="s">
+    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A81" s="17">
+        <v>10000</v>
+      </c>
+      <c r="B81" s="18">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A83" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="B78" s="10" t="s">
+      <c r="B83" s="10" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="79" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A79" s="11" t="s">
+    <row r="84" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A84" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="B79" s="12" t="s">
+      <c r="B84" s="12" t="s">
         <v>7</v>
-      </c>
-    </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A80" s="13">
-        <v>2</v>
-      </c>
-      <c r="B80" s="14">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A81" s="13">
-        <v>50</v>
-      </c>
-      <c r="B81" s="14">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A82" s="13">
-        <v>100</v>
-      </c>
-      <c r="B82" s="14">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A83" s="13">
-        <v>150</v>
-      </c>
-      <c r="B83" s="14">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A84" s="13">
-        <v>300</v>
-      </c>
-      <c r="B84" s="14">
-        <v>5</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A85" s="13">
-        <v>500</v>
+        <v>2</v>
       </c>
       <c r="B85" s="14">
-        <v>9</v>
+        <v>2</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A86" s="13">
-        <v>750</v>
+        <v>50</v>
       </c>
       <c r="B86" s="14">
-        <v>9</v>
+        <v>2</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A87" s="13">
-        <v>1000</v>
+        <v>100</v>
       </c>
       <c r="B87" s="14">
-        <v>16</v>
+        <v>3</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A88" s="13">
-        <v>1500</v>
+        <v>150</v>
       </c>
       <c r="B88" s="14">
-        <v>22</v>
+        <v>3</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A89" s="13">
-        <v>2000</v>
+        <v>300</v>
       </c>
       <c r="B89" s="14">
-        <v>27</v>
+        <v>5</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A90" s="13">
-        <v>2500</v>
+        <v>500</v>
       </c>
       <c r="B90" s="14">
-        <v>38</v>
+        <v>9</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A91" s="13">
+        <v>750</v>
+      </c>
+      <c r="B91" s="14">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A92" s="13">
+        <v>1000</v>
+      </c>
+      <c r="B92" s="14">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A93" s="13">
+        <v>1500</v>
+      </c>
+      <c r="B93" s="14">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A94" s="13">
+        <v>2000</v>
+      </c>
+      <c r="B94" s="14">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A95" s="13">
+        <v>2500</v>
+      </c>
+      <c r="B95" s="14">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A96" s="13">
         <v>5000</v>
       </c>
-      <c r="B91" s="14">
+      <c r="B96" s="14">
         <v>106</v>
       </c>
     </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A93" s="3" t="s">
+    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A97" s="13">
+        <v>10000</v>
+      </c>
+      <c r="B97" s="14">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A99" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B93" s="4" t="s">
+      <c r="B99" s="4" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="94" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A94" s="7" t="s">
+    <row r="100" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A100" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="B94" s="8" t="s">
+      <c r="B100" s="8" t="s">
         <v>7</v>
-      </c>
-    </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A95" s="5">
-        <v>2</v>
-      </c>
-      <c r="B95" s="6">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A96" s="5">
-        <v>50</v>
-      </c>
-      <c r="B96" s="6">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A97" s="5">
-        <v>100</v>
-      </c>
-      <c r="B97" s="6">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A98" s="5">
-        <v>150</v>
-      </c>
-      <c r="B98" s="6">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A99" s="5">
-        <v>300</v>
-      </c>
-      <c r="B99" s="6">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A100" s="5">
-        <v>500</v>
-      </c>
-      <c r="B100" s="6">
-        <v>9</v>
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A101" s="5">
-        <v>750</v>
+        <v>2</v>
       </c>
       <c r="B101" s="6">
-        <v>9</v>
+        <v>2</v>
       </c>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A102" s="5">
-        <v>1000</v>
+        <v>50</v>
       </c>
       <c r="B102" s="6">
-        <v>17</v>
+        <v>2</v>
       </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A103" s="5">
-        <v>1500</v>
+        <v>100</v>
       </c>
       <c r="B103" s="6">
-        <v>22</v>
+        <v>3</v>
       </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A104" s="5">
-        <v>2000</v>
+        <v>150</v>
       </c>
       <c r="B104" s="6">
-        <v>27</v>
+        <v>3</v>
       </c>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A105" s="5">
-        <v>2500</v>
+        <v>300</v>
       </c>
       <c r="B105" s="6">
-        <v>38</v>
+        <v>5</v>
       </c>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A106" s="5">
+        <v>500</v>
+      </c>
+      <c r="B106" s="6">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A107" s="5">
+        <v>750</v>
+      </c>
+      <c r="B107" s="6">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A108" s="5">
+        <v>1000</v>
+      </c>
+      <c r="B108" s="6">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A109" s="5">
+        <v>1500</v>
+      </c>
+      <c r="B109" s="6">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A110" s="5">
+        <v>2000</v>
+      </c>
+      <c r="B110" s="6">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A111" s="5">
+        <v>2500</v>
+      </c>
+      <c r="B111" s="6">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A112" s="5">
         <v>5000</v>
       </c>
-      <c r="B106" s="6">
+      <c r="B112" s="6">
         <v>106</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A113" s="5">
+        <v>10000</v>
+      </c>
+      <c r="B113" s="6">
+        <v>115</v>
       </c>
     </row>
   </sheetData>

</xml_diff>